<commit_message>
updated schema to 0.0.5
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/envelope_5_8.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/envelope_5_8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/vijay_tadimeti_pnnl_gov/Documents/Desktop/ruleset-checking-tool/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{8D3B01F6-3902-3B42-A670-5A83896CE454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C5CCF6E-FA91-814F-B4B5-2707F1A12393}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{8D3B01F6-3902-3B42-A670-5A83896CE454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5904B00D-CA4C-4848-A70D-D37886F2AD42}"/>
   <bookViews>
-    <workbookView xWindow="-35700" yWindow="840" windowWidth="32740" windowHeight="19420" activeTab="2" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="-35740" yWindow="460" windowWidth="32740" windowHeight="19420" activeTab="2" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="375">
   <si>
     <t>Rule ID</t>
   </si>
@@ -1091,9 +1091,6 @@
     <t>schema_version</t>
   </si>
   <si>
-    <t>0.0.1</t>
-  </si>
-  <si>
     <t>template_lookup</t>
   </si>
   <si>
@@ -1220,16 +1217,13 @@
     <t>false</t>
   </si>
   <si>
-    <t>template-rule-5-9-a</t>
-  </si>
-  <si>
-    <t>template-rule-5-9-b</t>
-  </si>
-  <si>
     <t>template-rule-5-10-a</t>
   </si>
   <si>
     <t>template-rule-5-10-b</t>
+  </si>
+  <si>
+    <t>0.0.5</t>
   </si>
 </sst>
 </file>
@@ -8255,8 +8249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B84DDF-E914-4844-8902-D6821C54B02C}">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10044,8 +10038,8 @@
   <dimension ref="A1:AM82"/>
   <sheetViews>
     <sheetView zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ2" sqref="AJ2"/>
+      <pane xSplit="3" topLeftCell="AI1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AI1" sqref="AI1:AI1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10170,17 +10164,13 @@
       <c r="AI1" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="AM1" s="5" t="s">
         <v>373</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="AM1" s="5" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
@@ -10275,12 +10265,8 @@
       <c r="AI2" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="AJ2" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="AK2" s="37" t="s">
-        <v>212</v>
-      </c>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
       <c r="AL2" s="37" t="s">
         <v>212</v>
       </c>
@@ -10382,12 +10368,8 @@
       <c r="AI3" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="AJ3" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="AK3" s="37" t="s">
-        <v>214</v>
-      </c>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
       <c r="AL3" s="37" t="s">
         <v>214</v>
       </c>
@@ -10489,12 +10471,8 @@
       <c r="AI4" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="AJ4" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="AK4" s="37" t="s">
-        <v>216</v>
-      </c>
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="37"/>
       <c r="AL4" s="37" t="s">
         <v>216</v>
       </c>
@@ -10686,12 +10664,8 @@
       <c r="AI7" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="AJ7" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="AK7" s="37" t="s">
-        <v>220</v>
-      </c>
+      <c r="AJ7" s="37"/>
+      <c r="AK7" s="37"/>
       <c r="AL7" s="37" t="s">
         <v>220</v>
       </c>
@@ -10928,12 +10902,8 @@
       <c r="AI11" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="AJ11" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="AK11" s="37" t="s">
-        <v>224</v>
-      </c>
+      <c r="AJ11" s="37"/>
+      <c r="AK11" s="37"/>
       <c r="AL11" s="37" t="s">
         <v>224</v>
       </c>
@@ -11548,12 +11518,8 @@
       <c r="AI21" s="37" t="s">
         <v>236</v>
       </c>
-      <c r="AJ21" s="37" t="s">
-        <v>236</v>
-      </c>
-      <c r="AK21" s="37" t="s">
-        <v>236</v>
-      </c>
+      <c r="AJ21" s="37"/>
+      <c r="AK21" s="37"/>
       <c r="AL21" s="37" t="s">
         <v>236</v>
       </c>
@@ -11690,12 +11656,8 @@
       <c r="AI23" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="AJ23" s="37" t="s">
-        <v>240</v>
-      </c>
-      <c r="AK23" s="37" t="s">
-        <v>240</v>
-      </c>
+      <c r="AJ23" s="37"/>
+      <c r="AK23" s="37"/>
       <c r="AL23" s="37" t="s">
         <v>239</v>
       </c>
@@ -11719,7 +11681,7 @@
       <c r="I24" s="37"/>
       <c r="J24" s="37"/>
       <c r="K24" s="109" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L24" s="37" t="b">
         <v>1</v>
@@ -11834,12 +11796,8 @@
       <c r="AI25" s="37">
         <v>90</v>
       </c>
-      <c r="AJ25" s="37">
-        <v>80</v>
-      </c>
-      <c r="AK25" s="37">
-        <v>80</v>
-      </c>
+      <c r="AJ25" s="37"/>
+      <c r="AK25" s="37"/>
       <c r="AL25" s="37">
         <v>90</v>
       </c>
@@ -12689,12 +12647,8 @@
       <c r="AI42" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="AJ42" s="37" t="s">
-        <v>260</v>
-      </c>
-      <c r="AK42" s="37" t="s">
-        <v>260</v>
-      </c>
+      <c r="AJ42" s="37"/>
+      <c r="AK42" s="37"/>
       <c r="AL42" s="37" t="s">
         <v>260</v>
       </c>
@@ -12923,12 +12877,8 @@
       <c r="AG46" s="37"/>
       <c r="AH46" s="37"/>
       <c r="AI46" s="37"/>
-      <c r="AJ46" s="37">
-        <v>1.5</v>
-      </c>
-      <c r="AK46" s="37">
-        <v>1.5</v>
-      </c>
+      <c r="AJ46" s="37"/>
+      <c r="AK46" s="37"/>
       <c r="AL46" s="37"/>
       <c r="AM46" s="37"/>
     </row>
@@ -17846,10 +17796,10 @@
   <dimension ref="A1:BZ129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF17" sqref="AF17"/>
+      <selection pane="bottomRight" activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18003,10 +17953,7 @@
         <f t="shared" ref="AJ1:AK1" si="7">"rule-"&amp;AJ2&amp;"-"&amp;AJ3&amp;"-"&amp;AJ4</f>
         <v>rule-5-8-f</v>
       </c>
-      <c r="AK1" s="58" t="str">
-        <f t="shared" ref="AK1" si="8">"rule-"&amp;AK2&amp;"-"&amp;AK3&amp;"-"&amp;AK4</f>
-        <v>rule-5-9-a</v>
-      </c>
+      <c r="AK1" s="58"/>
     </row>
     <row r="2" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
@@ -18101,9 +18048,7 @@
       <c r="AJ2" s="83">
         <v>5</v>
       </c>
-      <c r="AK2" s="83">
-        <v>5</v>
-      </c>
+      <c r="AK2" s="83"/>
     </row>
     <row r="3" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -18198,9 +18143,7 @@
       <c r="AJ3" s="83">
         <v>8</v>
       </c>
-      <c r="AK3" s="83">
-        <v>9</v>
-      </c>
+      <c r="AK3" s="83"/>
     </row>
     <row r="4" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -18295,9 +18238,7 @@
       <c r="AJ4" s="83" t="s">
         <v>306</v>
       </c>
-      <c r="AK4" s="83" t="s">
-        <v>301</v>
-      </c>
+      <c r="AK4" s="83"/>
     </row>
     <row r="5" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52" t="s">
@@ -18431,9 +18372,7 @@
       <c r="AJ6" s="81" t="s">
         <v>315</v>
       </c>
-      <c r="AK6" s="81" t="s">
-        <v>315</v>
-      </c>
+      <c r="AK6" s="81"/>
       <c r="AL6" s="81"/>
       <c r="AM6" s="81"/>
       <c r="AN6" s="81"/>
@@ -18569,9 +18508,7 @@
       <c r="AJ7" s="82" t="s">
         <v>318</v>
       </c>
-      <c r="AK7" s="82" t="s">
-        <v>318</v>
-      </c>
+      <c r="AK7" s="82"/>
     </row>
     <row r="8" spans="1:78" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -18588,117 +18525,114 @@
       <c r="H8" s="65"/>
       <c r="I8" s="68"/>
       <c r="J8" s="80" t="str">
-        <f t="shared" ref="J8:AD8" si="9">J2&amp;"-"&amp;J3</f>
+        <f t="shared" ref="J8:AD8" si="8">J2&amp;"-"&amp;J3</f>
         <v>5-2</v>
       </c>
       <c r="K8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-2</v>
       </c>
       <c r="L8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-3</v>
       </c>
       <c r="M8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-3</v>
       </c>
       <c r="N8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-4</v>
       </c>
       <c r="O8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-4</v>
       </c>
       <c r="P8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-5</v>
       </c>
       <c r="Q8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-5</v>
       </c>
       <c r="R8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-5</v>
       </c>
       <c r="S8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-5</v>
       </c>
       <c r="T8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-5</v>
       </c>
       <c r="U8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-5</v>
       </c>
       <c r="V8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-5</v>
       </c>
       <c r="W8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-6</v>
       </c>
       <c r="X8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-6</v>
       </c>
       <c r="Y8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-7</v>
       </c>
       <c r="Z8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-7</v>
       </c>
       <c r="AA8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-7</v>
       </c>
       <c r="AB8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-7</v>
       </c>
       <c r="AC8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-7</v>
       </c>
       <c r="AD8" s="80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5-7</v>
       </c>
       <c r="AE8" s="80" t="str">
-        <f t="shared" ref="AE8" si="10">AE2&amp;"-"&amp;AE3</f>
+        <f t="shared" ref="AE8" si="9">AE2&amp;"-"&amp;AE3</f>
         <v>5-8</v>
       </c>
       <c r="AF8" s="80" t="str">
-        <f t="shared" ref="AF8:AI8" si="11">AF2&amp;"-"&amp;AF3</f>
+        <f t="shared" ref="AF8:AI8" si="10">AF2&amp;"-"&amp;AF3</f>
         <v>5-8</v>
       </c>
       <c r="AG8" s="80" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>5-8</v>
       </c>
       <c r="AH8" s="80" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>5-8</v>
       </c>
       <c r="AI8" s="80" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>5-8</v>
       </c>
       <c r="AJ8" s="80" t="str">
         <f>AJ2&amp;"-"&amp;AJ3</f>
         <v>5-8</v>
       </c>
-      <c r="AK8" s="80" t="str">
-        <f>AK2&amp;"-"&amp;AK3</f>
-        <v>5-9</v>
-      </c>
+      <c r="AK8" s="80"/>
     </row>
     <row r="9" spans="1:78" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
@@ -18824,10 +18758,7 @@
         <f>INDEX(RulesTable[Ruleset Reference],MATCH(AJ$8,RulesTable[Rule ID],0))</f>
         <v>G3.1 #5 (b) Opaque assemblies used for new buildings, existing buildings, or additions ... shall match the appropriate assembly maximum U-factors in Tables G3.4-1 through G3.4-8:</v>
       </c>
-      <c r="AK9" s="77" t="str">
-        <f>INDEX(RulesTable[Ruleset Reference],MATCH(AK$8,RulesTable[Rule ID],0))</f>
-        <v>G3.1 #1 (a) The simulation model of the proposed design shall be consistent with the design documents…</v>
-      </c>
+      <c r="AK9" s="77"/>
     </row>
     <row r="10" spans="1:78" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
@@ -18951,10 +18882,7 @@
         <f>INDEX(RulesTable[Rule Description],MATCH(AJ$8,RulesTable[Rule ID],0))</f>
         <v>Baseline below-grade walls shall match the appropriate assembly maximum C-factors in Tables G3.4-1 through G3.4-8</v>
       </c>
-      <c r="AK10" s="77" t="str">
-        <f>INDEX(RulesTable[Rule Description],MATCH(AK$8,RulesTable[Rule ID],0))</f>
-        <v>Below-grade wall C-factor must be the same in the proposed model as in the user model</v>
-      </c>
+      <c r="AK10" s="77"/>
     </row>
     <row r="11" spans="1:78" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
@@ -19078,10 +19006,7 @@
         <f>INDEX(RulesTable[Applicable RMR],MATCH(AJ$8,RulesTable[Rule ID],0))</f>
         <v>Baseline RMR</v>
       </c>
-      <c r="AK11" s="77" t="str">
-        <f>INDEX(RulesTable[Applicable RMR],MATCH(AK$8,RulesTable[Rule ID],0))</f>
-        <v>Proposed RMR</v>
-      </c>
+      <c r="AK11" s="77"/>
     </row>
     <row r="12" spans="1:78" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
@@ -19205,10 +19130,7 @@
         <f>INDEX(RulesTable[Rule Assertion],MATCH(AJ$8,RulesTable[Rule ID],0))</f>
         <v>=</v>
       </c>
-      <c r="AK12" s="77" t="str">
-        <f>INDEX(RulesTable[Rule Assertion],MATCH(AK$8,RulesTable[Rule ID],0))</f>
-        <v>=</v>
-      </c>
+      <c r="AK12" s="77"/>
     </row>
     <row r="13" spans="1:78" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
@@ -19332,10 +19254,7 @@
         <f>INDEX(RulesTable[Comparison Value],MATCH(AJ$8,RulesTable[Rule ID],0))</f>
         <v>Expected Value</v>
       </c>
-      <c r="AK13" s="77" t="str">
-        <f>INDEX(RulesTable[Comparison Value],MATCH(AK$8,RulesTable[Rule ID],0))</f>
-        <v>User RMR</v>
-      </c>
+      <c r="AK13" s="77"/>
     </row>
     <row r="14" spans="1:78" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
@@ -19459,10 +19378,7 @@
         <f>INDEX(RulesTable[Rule Dependency],MATCH(AJ$8,RulesTable[Rule ID],0))</f>
         <v>None</v>
       </c>
-      <c r="AK14" s="77" t="str">
-        <f>INDEX(RulesTable[Rule Dependency],MATCH(AK$8,RulesTable[Rule ID],0))</f>
-        <v>None</v>
-      </c>
+      <c r="AK14" s="77"/>
     </row>
     <row r="15" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
@@ -19586,10 +19502,7 @@
         <f>INDEX(RulesTable[Mandatory Rule],MATCH(AJ$8,RulesTable[Rule ID],0))</f>
         <v>0</v>
       </c>
-      <c r="AK15" s="78">
-        <f>INDEX(RulesTable[Mandatory Rule],MATCH(AK$8,RulesTable[Rule ID],0))</f>
-        <v>0</v>
-      </c>
+      <c r="AK15" s="78"/>
     </row>
     <row r="16" spans="1:78" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="54" t="s">
@@ -19606,93 +19519,91 @@
       <c r="H16" s="71"/>
       <c r="I16" s="71"/>
       <c r="J16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="K16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="L16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="M16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="N16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="O16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="P16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="Q16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="R16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="S16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="T16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="U16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="V16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="W16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="X16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="Y16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="Z16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="AA16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="AB16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="AC16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="AD16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="AE16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="AF16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="AG16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="AH16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="AI16" s="82" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="AJ16" s="82" t="s">
-        <v>330</v>
-      </c>
-      <c r="AK16" s="82" t="s">
-        <v>330</v>
-      </c>
+        <v>374</v>
+      </c>
+      <c r="AK16" s="82"/>
     </row>
     <row r="17" spans="1:37" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="54" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B17" s="54"/>
       <c r="C17" s="55"/>
@@ -19783,16 +19694,14 @@
       <c r="AJ17" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="AK17" s="82" t="s">
-        <v>210</v>
-      </c>
+      <c r="AK17" s="82"/>
     </row>
     <row r="18" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>332</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>333</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -19802,124 +19711,121 @@
       <c r="H18" s="65"/>
       <c r="I18" s="65"/>
       <c r="J18" s="77" t="str">
-        <f t="shared" ref="J18:O18" si="12">IF(OR(J11="User RMR", J13="User RMR"),"true","")</f>
+        <f t="shared" ref="J18:O18" si="11">IF(OR(J11="User RMR", J13="User RMR"),"true","")</f>
         <v>true</v>
       </c>
       <c r="K18" s="77" t="str">
+        <f t="shared" si="11"/>
+        <v>true</v>
+      </c>
+      <c r="L18" s="77" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="M18" s="77" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="N18" s="77" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="O18" s="77" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="P18" s="77" t="str">
+        <f t="shared" ref="P18:Q18" si="12">IF(OR(P11="User RMR", P13="User RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="Q18" s="77" t="str">
         <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="R18" s="77" t="str">
+        <f t="shared" ref="R18:S18" si="13">IF(OR(R11="User RMR", R13="User RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="S18" s="77" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="T18" s="77" t="str">
+        <f t="shared" ref="T18:U18" si="14">IF(OR(T11="User RMR", T13="User RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="U18" s="77" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="V18" s="77" t="str">
+        <f t="shared" ref="V18:W18" si="15">IF(OR(V11="User RMR", V13="User RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="W18" s="77" t="str">
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
-      <c r="L18" s="77" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="M18" s="77" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="N18" s="77" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="O18" s="77" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="P18" s="77" t="str">
-        <f t="shared" ref="P18:Q18" si="13">IF(OR(P11="User RMR", P13="User RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="Q18" s="77" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="R18" s="77" t="str">
-        <f t="shared" ref="R18:S18" si="14">IF(OR(R11="User RMR", R13="User RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="S18" s="77" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="T18" s="77" t="str">
-        <f t="shared" ref="T18:U18" si="15">IF(OR(T11="User RMR", T13="User RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="U18" s="77" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="V18" s="77" t="str">
-        <f t="shared" ref="V18:W18" si="16">IF(OR(V11="User RMR", V13="User RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="W18" s="77" t="str">
+      <c r="X18" s="77" t="str">
+        <f t="shared" ref="X18:Y18" si="16">IF(OR(X11="User RMR", X13="User RMR"),"true","")</f>
+        <v>true</v>
+      </c>
+      <c r="Y18" s="77" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
-      </c>
-      <c r="X18" s="77" t="str">
-        <f t="shared" ref="X18:Y18" si="17">IF(OR(X11="User RMR", X13="User RMR"),"true","")</f>
-        <v>true</v>
-      </c>
-      <c r="Y18" s="77" t="str">
+        <v/>
+      </c>
+      <c r="Z18" s="77" t="str">
+        <f t="shared" ref="Z18:AA18" si="17">IF(OR(Z11="User RMR", Z13="User RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="AA18" s="77" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="Z18" s="77" t="str">
-        <f t="shared" ref="Z18:AA18" si="18">IF(OR(Z11="User RMR", Z13="User RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="AA18" s="77" t="str">
+      <c r="AB18" s="77" t="str">
+        <f t="shared" ref="AB18:AC18" si="18">IF(OR(AB11="User RMR", AB13="User RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="AC18" s="77" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="AB18" s="77" t="str">
-        <f t="shared" ref="AB18:AC18" si="19">IF(OR(AB11="User RMR", AB13="User RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="AC18" s="77" t="str">
+      <c r="AD18" s="77" t="str">
+        <f t="shared" ref="AD18:AJ18" si="19">IF(OR(AD11="User RMR", AD13="User RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="AE18" s="77" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
-      <c r="AD18" s="77" t="str">
-        <f t="shared" ref="AD18:AJ18" si="20">IF(OR(AD11="User RMR", AD13="User RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="AE18" s="77" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
       <c r="AF18" s="77" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AG18" s="77" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AH18" s="77" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AI18" s="77" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AJ18" s="77" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="AK18" s="77" t="str">
-        <f t="shared" ref="AK18" si="21">IF(OR(AK11="User RMR", AK13="User RMR"),"true","")</f>
-        <v>true</v>
-      </c>
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="AK18" s="77"/>
     </row>
     <row r="19" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -19929,124 +19835,121 @@
       <c r="H19" s="65"/>
       <c r="I19" s="65"/>
       <c r="J19" s="77" t="str">
-        <f t="shared" ref="J19:O19" si="22">IF(OR(J11="Proposed RMR", J13="Proposed RMR"),"true","")</f>
+        <f t="shared" ref="J19:O19" si="20">IF(OR(J11="Proposed RMR", J13="Proposed RMR"),"true","")</f>
         <v>true</v>
       </c>
       <c r="K19" s="77" t="str">
+        <f t="shared" si="20"/>
+        <v>true</v>
+      </c>
+      <c r="L19" s="77" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="M19" s="77" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="N19" s="77" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O19" s="77" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="P19" s="77" t="str">
+        <f t="shared" ref="P19:Q19" si="21">IF(OR(P11="Proposed RMR", P13="Proposed RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="Q19" s="77" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="R19" s="77" t="str">
+        <f t="shared" ref="R19:S19" si="22">IF(OR(R11="Proposed RMR", R13="Proposed RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="S19" s="77" t="str">
         <f t="shared" si="22"/>
+        <v/>
+      </c>
+      <c r="T19" s="77" t="str">
+        <f t="shared" ref="T19:U19" si="23">IF(OR(T11="Proposed RMR", T13="Proposed RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="U19" s="77" t="str">
+        <f t="shared" si="23"/>
+        <v/>
+      </c>
+      <c r="V19" s="77" t="str">
+        <f t="shared" ref="V19:W19" si="24">IF(OR(V11="Proposed RMR", V13="Proposed RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="W19" s="77" t="str">
+        <f t="shared" si="24"/>
         <v>true</v>
       </c>
-      <c r="L19" s="77" t="str">
-        <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="M19" s="77" t="str">
-        <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="N19" s="77" t="str">
-        <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="O19" s="77" t="str">
-        <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="P19" s="77" t="str">
-        <f t="shared" ref="P19:Q19" si="23">IF(OR(P11="Proposed RMR", P13="Proposed RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="Q19" s="77" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-      <c r="R19" s="77" t="str">
-        <f t="shared" ref="R19:S19" si="24">IF(OR(R11="Proposed RMR", R13="Proposed RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="S19" s="77" t="str">
-        <f t="shared" si="24"/>
-        <v/>
-      </c>
-      <c r="T19" s="77" t="str">
-        <f t="shared" ref="T19:U19" si="25">IF(OR(T11="Proposed RMR", T13="Proposed RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="U19" s="77" t="str">
+      <c r="X19" s="77" t="str">
+        <f t="shared" ref="X19:Y19" si="25">IF(OR(X11="Proposed RMR", X13="Proposed RMR"),"true","")</f>
+        <v>true</v>
+      </c>
+      <c r="Y19" s="77" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="V19" s="77" t="str">
-        <f t="shared" ref="V19:W19" si="26">IF(OR(V11="Proposed RMR", V13="Proposed RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="W19" s="77" t="str">
+      <c r="Z19" s="77" t="str">
+        <f t="shared" ref="Z19:AA19" si="26">IF(OR(Z11="Proposed RMR", Z13="Proposed RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="AA19" s="77" t="str">
         <f t="shared" si="26"/>
-        <v>true</v>
-      </c>
-      <c r="X19" s="77" t="str">
-        <f t="shared" ref="X19:Y19" si="27">IF(OR(X11="Proposed RMR", X13="Proposed RMR"),"true","")</f>
-        <v>true</v>
-      </c>
-      <c r="Y19" s="77" t="str">
+        <v/>
+      </c>
+      <c r="AB19" s="77" t="str">
+        <f t="shared" ref="AB19:AC19" si="27">IF(OR(AB11="Proposed RMR", AB13="Proposed RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="AC19" s="77" t="str">
         <f t="shared" si="27"/>
         <v/>
       </c>
-      <c r="Z19" s="77" t="str">
-        <f t="shared" ref="Z19:AA19" si="28">IF(OR(Z11="Proposed RMR", Z13="Proposed RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="AA19" s="77" t="str">
+      <c r="AD19" s="77" t="str">
+        <f t="shared" ref="AD19:AJ19" si="28">IF(OR(AD11="Proposed RMR", AD13="Proposed RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="AE19" s="77" t="str">
         <f t="shared" si="28"/>
         <v/>
       </c>
-      <c r="AB19" s="77" t="str">
-        <f t="shared" ref="AB19:AC19" si="29">IF(OR(AB11="Proposed RMR", AB13="Proposed RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="AC19" s="77" t="str">
-        <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="AD19" s="77" t="str">
-        <f t="shared" ref="AD19:AJ19" si="30">IF(OR(AD11="Proposed RMR", AD13="Proposed RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="AE19" s="77" t="str">
-        <f t="shared" si="30"/>
-        <v/>
-      </c>
       <c r="AF19" s="77" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AG19" s="77" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AH19" s="77" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AI19" s="77" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AJ19" s="77" t="str">
-        <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="AK19" s="77" t="str">
-        <f t="shared" ref="AK19" si="31">IF(OR(AK11="Proposed RMR", AK13="Proposed RMR"),"true","")</f>
-        <v>true</v>
-      </c>
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="AK19" s="77"/>
     </row>
     <row r="20" spans="1:37" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -20056,124 +19959,121 @@
       <c r="H20" s="67"/>
       <c r="I20" s="67"/>
       <c r="J20" s="84" t="str">
-        <f t="shared" ref="J20:O20" si="32">IF(OR(J11="Baseline RMR", J13="Baseline RMR"),"true","")</f>
+        <f t="shared" ref="J20:O20" si="29">IF(OR(J11="Baseline RMR", J13="Baseline RMR"),"true","")</f>
         <v/>
       </c>
       <c r="K20" s="84" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="L20" s="84" t="str">
+        <f t="shared" si="29"/>
+        <v>true</v>
+      </c>
+      <c r="M20" s="84" t="str">
+        <f t="shared" si="29"/>
+        <v>true</v>
+      </c>
+      <c r="N20" s="84" t="str">
+        <f t="shared" si="29"/>
+        <v>true</v>
+      </c>
+      <c r="O20" s="84" t="str">
+        <f t="shared" si="29"/>
+        <v>true</v>
+      </c>
+      <c r="P20" s="84" t="str">
+        <f t="shared" ref="P20:Q20" si="30">IF(OR(P11="Baseline RMR", P13="Baseline RMR"),"true","")</f>
+        <v>true</v>
+      </c>
+      <c r="Q20" s="84" t="str">
+        <f t="shared" si="30"/>
+        <v>true</v>
+      </c>
+      <c r="R20" s="84" t="str">
+        <f t="shared" ref="R20:S20" si="31">IF(OR(R11="Baseline RMR", R13="Baseline RMR"),"true","")</f>
+        <v>true</v>
+      </c>
+      <c r="S20" s="84" t="str">
+        <f t="shared" si="31"/>
+        <v>true</v>
+      </c>
+      <c r="T20" s="84" t="str">
+        <f t="shared" ref="T20:U20" si="32">IF(OR(T11="Baseline RMR", T13="Baseline RMR"),"true","")</f>
+        <v>true</v>
+      </c>
+      <c r="U20" s="84" t="str">
         <f t="shared" si="32"/>
         <v>true</v>
       </c>
-      <c r="M20" s="84" t="str">
-        <f t="shared" si="32"/>
+      <c r="V20" s="84" t="str">
+        <f t="shared" ref="V20:W20" si="33">IF(OR(V11="Baseline RMR", V13="Baseline RMR"),"true","")</f>
         <v>true</v>
       </c>
-      <c r="N20" s="84" t="str">
-        <f t="shared" si="32"/>
-        <v>true</v>
-      </c>
-      <c r="O20" s="84" t="str">
-        <f t="shared" si="32"/>
-        <v>true</v>
-      </c>
-      <c r="P20" s="84" t="str">
-        <f t="shared" ref="P20:Q20" si="33">IF(OR(P11="Baseline RMR", P13="Baseline RMR"),"true","")</f>
-        <v>true</v>
-      </c>
-      <c r="Q20" s="84" t="str">
+      <c r="W20" s="84" t="str">
         <f t="shared" si="33"/>
-        <v>true</v>
-      </c>
-      <c r="R20" s="84" t="str">
-        <f t="shared" ref="R20:S20" si="34">IF(OR(R11="Baseline RMR", R13="Baseline RMR"),"true","")</f>
-        <v>true</v>
-      </c>
-      <c r="S20" s="84" t="str">
+        <v/>
+      </c>
+      <c r="X20" s="84" t="str">
+        <f t="shared" ref="X20:Y20" si="34">IF(OR(X11="Baseline RMR", X13="Baseline RMR"),"true","")</f>
+        <v/>
+      </c>
+      <c r="Y20" s="84" t="str">
         <f t="shared" si="34"/>
         <v>true</v>
       </c>
-      <c r="T20" s="84" t="str">
-        <f t="shared" ref="T20:U20" si="35">IF(OR(T11="Baseline RMR", T13="Baseline RMR"),"true","")</f>
+      <c r="Z20" s="84" t="str">
+        <f t="shared" ref="Z20:AA20" si="35">IF(OR(Z11="Baseline RMR", Z13="Baseline RMR"),"true","")</f>
         <v>true</v>
       </c>
-      <c r="U20" s="84" t="str">
+      <c r="AA20" s="84" t="str">
         <f t="shared" si="35"/>
         <v>true</v>
       </c>
-      <c r="V20" s="84" t="str">
-        <f t="shared" ref="V20:W20" si="36">IF(OR(V11="Baseline RMR", V13="Baseline RMR"),"true","")</f>
+      <c r="AB20" s="84" t="str">
+        <f t="shared" ref="AB20:AC20" si="36">IF(OR(AB11="Baseline RMR", AB13="Baseline RMR"),"true","")</f>
         <v>true</v>
       </c>
-      <c r="W20" s="84" t="str">
+      <c r="AC20" s="84" t="str">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-      <c r="X20" s="84" t="str">
-        <f t="shared" ref="X20:Y20" si="37">IF(OR(X11="Baseline RMR", X13="Baseline RMR"),"true","")</f>
-        <v/>
-      </c>
-      <c r="Y20" s="84" t="str">
+        <v>true</v>
+      </c>
+      <c r="AD20" s="84" t="str">
+        <f t="shared" ref="AD20:AJ20" si="37">IF(OR(AD11="Baseline RMR", AD13="Baseline RMR"),"true","")</f>
+        <v>true</v>
+      </c>
+      <c r="AE20" s="84" t="str">
         <f t="shared" si="37"/>
         <v>true</v>
       </c>
-      <c r="Z20" s="84" t="str">
-        <f t="shared" ref="Z20:AA20" si="38">IF(OR(Z11="Baseline RMR", Z13="Baseline RMR"),"true","")</f>
+      <c r="AF20" s="84" t="str">
+        <f t="shared" si="37"/>
         <v>true</v>
       </c>
-      <c r="AA20" s="84" t="str">
-        <f t="shared" si="38"/>
+      <c r="AG20" s="84" t="str">
+        <f t="shared" si="37"/>
         <v>true</v>
       </c>
-      <c r="AB20" s="84" t="str">
-        <f t="shared" ref="AB20:AC20" si="39">IF(OR(AB11="Baseline RMR", AB13="Baseline RMR"),"true","")</f>
+      <c r="AH20" s="84" t="str">
+        <f t="shared" si="37"/>
         <v>true</v>
       </c>
-      <c r="AC20" s="84" t="str">
-        <f t="shared" si="39"/>
+      <c r="AI20" s="84" t="str">
+        <f t="shared" si="37"/>
         <v>true</v>
       </c>
-      <c r="AD20" s="84" t="str">
-        <f t="shared" ref="AD20:AJ20" si="40">IF(OR(AD11="Baseline RMR", AD13="Baseline RMR"),"true","")</f>
+      <c r="AJ20" s="84" t="str">
+        <f t="shared" si="37"/>
         <v>true</v>
       </c>
-      <c r="AE20" s="84" t="str">
-        <f t="shared" si="40"/>
-        <v>true</v>
-      </c>
-      <c r="AF20" s="84" t="str">
-        <f t="shared" si="40"/>
-        <v>true</v>
-      </c>
-      <c r="AG20" s="84" t="str">
-        <f t="shared" si="40"/>
-        <v>true</v>
-      </c>
-      <c r="AH20" s="84" t="str">
-        <f t="shared" si="40"/>
-        <v>true</v>
-      </c>
-      <c r="AI20" s="84" t="str">
-        <f t="shared" si="40"/>
-        <v>true</v>
-      </c>
-      <c r="AJ20" s="84" t="str">
-        <f t="shared" si="40"/>
-        <v>true</v>
-      </c>
-      <c r="AK20" s="84" t="str">
-        <f t="shared" ref="AK20" si="41">IF(OR(AK11="Baseline RMR", AK13="Baseline RMR"),"true","")</f>
-        <v/>
-      </c>
+      <c r="AK20" s="84"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C21" s="96" t="str" cm="1">
         <f t="array" ref="C21">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -20311,17 +20211,14 @@
         <f t="array" ref="AJ21">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v>ashrae_229</v>
       </c>
-      <c r="AK21" s="79" t="str" cm="1">
-        <f t="array" ref="AK21">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v>ashrae_229</v>
-      </c>
+      <c r="AK21" s="79"/>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C22" s="96" t="str" cm="1">
         <f t="array" ref="C22">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -20459,17 +20356,14 @@
         <f t="array" ref="AJ22">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v>building_1</v>
       </c>
-      <c r="AK22" s="79" t="str" cm="1">
-        <f t="array" ref="AK22">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v>building_1</v>
-      </c>
+      <c r="AK22" s="79"/>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C23" s="96" t="str" cm="1">
         <f t="array" ref="C23">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -20607,17 +20501,14 @@
         <f t="array" ref="AJ23">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v>schedule_1</v>
       </c>
-      <c r="AK23" s="79" t="str" cm="1">
-        <f t="array" ref="AK23">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v>schedule_1</v>
-      </c>
+      <c r="AK23" s="79"/>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C24" s="96" t="str" cm="1">
         <f t="array" ref="C24">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -20755,17 +20646,14 @@
         <f t="array" ref="AJ24">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK24" s="79" t="str" cm="1">
-        <f t="array" ref="AK24">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK24" s="79"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C25" s="96" t="str" cm="1">
         <f t="array" ref="C25">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -20903,17 +20791,14 @@
         <f t="array" ref="AJ25">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK25" s="79" t="str" cm="1">
-        <f t="array" ref="AK25">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK25" s="79"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C26" s="96" t="str" cm="1">
         <f t="array" ref="C26">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -21051,17 +20936,14 @@
         <f t="array" ref="AJ26">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v>segment_1</v>
       </c>
-      <c r="AK26" s="79" t="str" cm="1">
-        <f t="array" ref="AK26">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v>segment_1</v>
-      </c>
+      <c r="AK26" s="79"/>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C27" s="96" t="str" cm="1">
         <f t="array" ref="C27">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -21199,17 +21081,14 @@
         <f t="array" ref="AJ27">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK27" s="79" t="str" cm="1">
-        <f t="array" ref="AK27">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK27" s="79"/>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C28" s="96" t="str" cm="1">
         <f t="array" ref="C28">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -21347,17 +21226,14 @@
         <f t="array" ref="AJ28">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK28" s="79" t="str" cm="1">
-        <f t="array" ref="AK28">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK28" s="79"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C29" s="96" t="str" cm="1">
         <f t="array" ref="C29">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -21495,17 +21371,14 @@
         <f t="array" ref="AJ29">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK29" s="79" t="str" cm="1">
-        <f t="array" ref="AK29">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK29" s="79"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C30" s="96" t="str" cm="1">
         <f t="array" ref="C30">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -21643,17 +21516,14 @@
         <f t="array" ref="AJ30">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v>zone_1</v>
       </c>
-      <c r="AK30" s="79" t="str" cm="1">
-        <f t="array" ref="AK30">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v>zone_1</v>
-      </c>
+      <c r="AK30" s="79"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C31" s="96" t="str" cm="1">
         <f t="array" ref="C31">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -21791,17 +21661,14 @@
         <f t="array" ref="AJ31">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v>schedule_1</v>
       </c>
-      <c r="AK31" s="79" t="str" cm="1">
-        <f t="array" ref="AK31">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v>schedule_1</v>
-      </c>
+      <c r="AK31" s="79"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C32" s="96" t="str" cm="1">
         <f t="array" ref="C32">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -21939,17 +21806,14 @@
         <f t="array" ref="AJ32">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v>schedule_1</v>
       </c>
-      <c r="AK32" s="79" t="str" cm="1">
-        <f t="array" ref="AK32">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v>schedule_1</v>
-      </c>
+      <c r="AK32" s="79"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C33" s="96" t="str" cm="1">
         <f t="array" ref="C33">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -22088,17 +21952,14 @@
         <f t="array" ref="AJ33">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK33" s="79" t="str" cm="1">
-        <f t="array" ref="AK33">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK33" s="79"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C34" s="96" t="str" cm="1">
         <f t="array" ref="C34">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -22236,17 +22097,14 @@
         <f t="array" ref="AJ34">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK34" s="79" t="str" cm="1">
-        <f t="array" ref="AK34">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK34" s="79"/>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C35" s="96" t="str" cm="1">
         <f t="array" ref="C35">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -22384,17 +22242,14 @@
         <f t="array" ref="AJ35">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK35" s="79" t="str" cm="1">
-        <f t="array" ref="AK35">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK35" s="79"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C36" s="96" t="str" cm="1">
         <f t="array" ref="C36">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -22532,17 +22387,14 @@
         <f t="array" ref="AJ36">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK36" s="79" t="str" cm="1">
-        <f t="array" ref="AK36">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK36" s="79"/>
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C37" s="96" t="str" cm="1">
         <f t="array" ref="C37">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -22680,17 +22532,14 @@
         <f t="array" ref="AJ37">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK37" s="79" t="str" cm="1">
-        <f t="array" ref="AK37">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK37" s="79"/>
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C38" s="96" t="str" cm="1">
         <f t="array" ref="C38">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -22828,17 +22677,14 @@
         <f t="array" ref="AJ38">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK38" s="79" t="str" cm="1">
-        <f t="array" ref="AK38">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK38" s="79"/>
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C39" s="96" t="str" cm="1">
         <f t="array" ref="C39">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -22976,17 +22822,14 @@
         <f t="array" ref="AJ39">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK39" s="79" t="str" cm="1">
-        <f t="array" ref="AK39">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK39" s="79"/>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C40" s="96" t="str" cm="1">
         <f t="array" ref="C40">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -23124,17 +22967,14 @@
         <f t="array" ref="AJ40">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v>surface_1</v>
       </c>
-      <c r="AK40" s="79" t="str" cm="1">
-        <f t="array" ref="AK40">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v>surface_1</v>
-      </c>
+      <c r="AK40" s="79"/>
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C41" s="96" t="str" cm="1">
         <f t="array" ref="C41">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -23272,17 +23112,14 @@
         <f t="array" ref="AJ41">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK41" s="79" t="str" cm="1">
-        <f t="array" ref="AK41">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK41" s="79"/>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C42" s="96" t="str" cm="1">
         <f t="array" ref="C42">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -23420,17 +23257,14 @@
         <f t="array" ref="AJ42">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v>GROUND</v>
       </c>
-      <c r="AK42" s="79" t="str" cm="1">
-        <f t="array" ref="AK42">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v>GROUND</v>
-      </c>
+      <c r="AK42" s="79"/>
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C43" s="96" t="str" cm="1">
         <f t="array" ref="C43">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -23568,17 +23402,14 @@
         <f t="array" ref="AJ43">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK43" s="79" t="str" cm="1">
-        <f t="array" ref="AK43">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK43" s="79"/>
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C44" s="96" t="str" cm="1">
         <f t="array" ref="C44">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -23716,17 +23547,14 @@
         <f t="array" ref="AJ44">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v>90</v>
       </c>
-      <c r="AK44" s="79" cm="1">
-        <f t="array" ref="AK44">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v>90</v>
-      </c>
+      <c r="AK44" s="79"/>
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C45" s="96" t="str" cm="1">
         <f t="array" ref="C45">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -23864,17 +23692,14 @@
         <f t="array" ref="AJ45">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK45" s="79" t="str" cm="1">
-        <f t="array" ref="AK45">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK45" s="79"/>
     </row>
     <row r="46" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C46" s="96" t="str" cm="1">
         <f t="array" ref="C46">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -24012,17 +23837,14 @@
         <f t="array" ref="AJ46">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK46" s="79" t="str" cm="1">
-        <f t="array" ref="AK46">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK46" s="79"/>
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C47" s="96" t="str" cm="1">
         <f t="array" ref="C47">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -24160,17 +23982,14 @@
         <f t="array" ref="AJ47">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK47" s="79" t="str" cm="1">
-        <f t="array" ref="AK47">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK47" s="79"/>
     </row>
     <row r="48" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C48" s="96" t="str" cm="1">
         <f t="array" ref="C48">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -24308,17 +24127,14 @@
         <f t="array" ref="AJ48">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK48" s="79" t="str" cm="1">
-        <f t="array" ref="AK48">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK48" s="79"/>
     </row>
     <row r="49" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C49" s="96" t="str" cm="1">
         <f t="array" ref="C49">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -24456,17 +24272,14 @@
         <f t="array" ref="AJ49">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK49" s="79" t="str" cm="1">
-        <f t="array" ref="AK49">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK49" s="79"/>
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C50" s="96" t="str" cm="1">
         <f t="array" ref="C50">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -24604,17 +24417,14 @@
         <f t="array" ref="AJ50">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK50" s="79" t="str" cm="1">
-        <f t="array" ref="AK50">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK50" s="79"/>
     </row>
     <row r="51" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C51" s="96" t="str" cm="1">
         <f t="array" ref="C51">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -24752,17 +24562,14 @@
         <f t="array" ref="AJ51">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK51" s="79" t="str" cm="1">
-        <f t="array" ref="AK51">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK51" s="79"/>
     </row>
     <row r="52" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C52" s="96" t="str" cm="1">
         <f t="array" ref="C52">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -24900,17 +24707,14 @@
         <f t="array" ref="AJ52">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK52" s="79" t="str" cm="1">
-        <f t="array" ref="AK52">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK52" s="79"/>
     </row>
     <row r="53" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C53" s="96" t="str" cm="1">
         <f t="array" ref="C53">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25048,17 +24852,14 @@
         <f t="array" ref="AJ53">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK53" s="79" t="str" cm="1">
-        <f t="array" ref="AK53">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK53" s="79"/>
     </row>
     <row r="54" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C54" s="96" t="str" cm="1">
         <f t="array" ref="C54">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25196,17 +24997,14 @@
         <f t="array" ref="AJ54">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK54" s="79" t="str" cm="1">
-        <f t="array" ref="AK54">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK54" s="79"/>
     </row>
     <row r="55" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C55" s="96" t="str" cm="1">
         <f t="array" ref="C55">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25344,17 +25142,14 @@
         <f t="array" ref="AJ55">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK55" s="79" t="str" cm="1">
-        <f t="array" ref="AK55">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK55" s="79"/>
     </row>
     <row r="56" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C56" s="96" t="str" cm="1">
         <f t="array" ref="C56">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25403,10 +25198,10 @@
     </row>
     <row r="57" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C57" s="96" t="str" cm="1">
         <f t="array" ref="C57">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25455,10 +25250,10 @@
     </row>
     <row r="58" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C58" s="96" t="str" cm="1">
         <f t="array" ref="C58">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25507,10 +25302,10 @@
     </row>
     <row r="59" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C59" s="96" t="str" cm="1">
         <f t="array" ref="C59">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25559,10 +25354,10 @@
     </row>
     <row r="60" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C60" s="96" t="str" cm="1">
         <f t="array" ref="C60">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25611,10 +25406,10 @@
     </row>
     <row r="61" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C61" s="96" t="str" cm="1">
         <f t="array" ref="C61">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25669,10 +25464,10 @@
     </row>
     <row r="62" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C62" s="96" t="str" cm="1">
         <f t="array" ref="C62">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25723,10 +25518,10 @@
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C63" s="96" t="str" cm="1">
         <f t="array" ref="C63">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25775,10 +25570,10 @@
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C64" s="96" t="str" cm="1">
         <f t="array" ref="C64">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25827,10 +25622,10 @@
     </row>
     <row r="65" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C65" s="96" t="str" cm="1">
         <f t="array" ref="C65">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25879,10 +25674,10 @@
     </row>
     <row r="66" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C66" s="96" t="str" cm="1">
         <f t="array" ref="C66">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25931,10 +25726,10 @@
     </row>
     <row r="67" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C67" s="96" t="str" cm="1">
         <f t="array" ref="C67">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -25983,10 +25778,10 @@
     </row>
     <row r="68" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C68" s="96" t="str" cm="1">
         <f t="array" ref="C68">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26035,10 +25830,10 @@
     </row>
     <row r="69" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C69" s="96" t="str" cm="1">
         <f t="array" ref="C69">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26087,10 +25882,10 @@
     </row>
     <row r="70" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C70" s="96" t="str" cm="1">
         <f t="array" ref="C70">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26139,10 +25934,10 @@
     </row>
     <row r="71" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C71" s="96" t="str" cm="1">
         <f t="array" ref="C71">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26191,10 +25986,10 @@
     </row>
     <row r="72" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C72" s="96" t="str" cm="1">
         <f t="array" ref="C72">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26243,10 +26038,10 @@
     </row>
     <row r="73" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C73" s="96" t="str" cm="1">
         <f t="array" ref="C73">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26295,10 +26090,10 @@
     </row>
     <row r="74" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C74" s="96" t="str" cm="1">
         <f t="array" ref="C74">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26347,10 +26142,10 @@
     </row>
     <row r="75" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C75" s="96" t="str" cm="1">
         <f t="array" ref="C75">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26399,10 +26194,10 @@
     </row>
     <row r="76" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C76" s="96" t="str" cm="1">
         <f t="array" ref="C76">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26451,10 +26246,10 @@
     </row>
     <row r="77" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C77" s="96" t="str" cm="1">
         <f t="array" ref="C77">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26503,10 +26298,10 @@
     </row>
     <row r="78" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C78" s="96" t="str" cm="1">
         <f t="array" ref="C78">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26555,10 +26350,10 @@
     </row>
     <row r="79" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C79" s="96" t="str" cm="1">
         <f t="array" ref="C79">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26607,10 +26402,10 @@
     </row>
     <row r="80" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C80" s="96" t="str" cm="1">
         <f t="array" ref="C80">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26659,10 +26454,10 @@
     </row>
     <row r="81" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C81" s="96" t="str" cm="1">
         <f t="array" ref="C81">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26711,10 +26506,10 @@
     </row>
     <row r="82" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C82" s="96" t="str" cm="1">
         <f t="array" ref="C82">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26763,10 +26558,10 @@
     </row>
     <row r="83" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C83" s="96" t="str" cm="1">
         <f t="array" ref="C83">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26815,10 +26610,10 @@
     </row>
     <row r="84" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C84" s="96" t="str" cm="1">
         <f t="array" ref="C84">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26867,10 +26662,10 @@
     </row>
     <row r="85" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C85" s="96" t="str" cm="1">
         <f t="array" ref="C85">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26919,10 +26714,10 @@
     </row>
     <row r="86" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C86" s="96" t="str" cm="1">
         <f t="array" ref="C86">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -26971,10 +26766,10 @@
     </row>
     <row r="87" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C87" s="96" t="str" cm="1">
         <f t="array" ref="C87">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27023,10 +26818,10 @@
     </row>
     <row r="88" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C88" s="96" t="str" cm="1">
         <f t="array" ref="C88">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27075,10 +26870,10 @@
     </row>
     <row r="89" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C89" s="96" t="str" cm="1">
         <f t="array" ref="C89">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27127,10 +26922,10 @@
     </row>
     <row r="90" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C90" s="96" t="str" cm="1">
         <f t="array" ref="C90">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27179,10 +26974,10 @@
     </row>
     <row r="91" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C91" s="96" t="str" cm="1">
         <f t="array" ref="C91">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27231,10 +27026,10 @@
     </row>
     <row r="92" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C92" s="96" t="str" cm="1">
         <f t="array" ref="C92">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27283,10 +27078,10 @@
     </row>
     <row r="93" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C93" s="96" t="str" cm="1">
         <f t="array" ref="C93">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27335,10 +27130,10 @@
     </row>
     <row r="94" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C94" s="96" t="str" cm="1">
         <f t="array" ref="C94">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27387,10 +27182,10 @@
     </row>
     <row r="95" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C95" s="96" t="str" cm="1">
         <f t="array" ref="C95">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27439,10 +27234,10 @@
     </row>
     <row r="96" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C96" s="96" t="str" cm="1">
         <f t="array" ref="C96">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27491,10 +27286,10 @@
     </row>
     <row r="97" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C97" s="96" t="str" cm="1">
         <f t="array" ref="C97">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27543,10 +27338,10 @@
     </row>
     <row r="98" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C98" s="96" t="str" cm="1">
         <f t="array" ref="C98">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27595,10 +27390,10 @@
     </row>
     <row r="99" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C99" s="96" t="str" cm="1">
         <f t="array" ref="C99">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27647,10 +27442,10 @@
     </row>
     <row r="100" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C100" s="96" t="str" cm="1">
         <f t="array" ref="C100">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27699,10 +27494,10 @@
     </row>
     <row r="101" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C101" s="96" t="str" cm="1">
         <f t="array" ref="C101">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27751,10 +27546,10 @@
     </row>
     <row r="102" spans="1:37" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="54" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B102" s="55" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C102" s="98" t="str" cm="1">
         <f t="array" ref="C102">IF(INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1)="","",INDEX(Templates!A$2:A$142,ROW()-ROW($21:$21)+1))</f>
@@ -27880,17 +27675,14 @@
         <f t="array" ref="AJ102">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AJ$21)+1, MATCH(AJ$17,Templates!$I$1:AI$1,0)))</f>
         <v/>
       </c>
-      <c r="AK102" s="108" t="str" cm="1">
-        <f t="array" ref="AK102">IF(INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0))="","",INDEX(Templates!$I$2:$AI$133,ROW()-ROW(AK$21)+1, MATCH(AK$17,Templates!$I$1:AJ$1,0)))</f>
-        <v/>
-      </c>
+      <c r="AK102" s="108"/>
     </row>
     <row r="103" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C103" s="11" t="s">
         <v>235</v>
@@ -27936,10 +27728,10 @@
     </row>
     <row r="104" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C104" s="11" t="s">
         <v>259</v>
@@ -27987,10 +27779,10 @@
     </row>
     <row r="105" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C105" s="11" t="s">
         <v>259</v>
@@ -28073,10 +27865,10 @@
     </row>
     <row r="107" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C107" s="11" t="s">
         <v>235</v>
@@ -28122,10 +27914,10 @@
     </row>
     <row r="108" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C108" s="11" t="s">
         <v>259</v>
@@ -28173,10 +27965,10 @@
     </row>
     <row r="109" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C109" s="11" t="s">
         <v>259</v>
@@ -28220,10 +28012,10 @@
     </row>
     <row r="110" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C110" s="11" t="s">
         <v>259</v>
@@ -28267,10 +28059,10 @@
     </row>
     <row r="111" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C111" s="11" t="s">
         <v>259</v>
@@ -28314,10 +28106,10 @@
     </row>
     <row r="112" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C112" s="11" t="s">
         <v>235</v>
@@ -28363,10 +28155,10 @@
     </row>
     <row r="113" spans="1:37" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="54" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B113" s="55" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C113" s="55" t="s">
         <v>235</v>
@@ -28412,10 +28204,10 @@
     </row>
     <row r="114" spans="1:37" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C114" s="11" t="s">
         <v>259</v>
@@ -28461,10 +28253,10 @@
     </row>
     <row r="115" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C115" s="11" t="s">
         <v>259</v>
@@ -28508,10 +28300,10 @@
     </row>
     <row r="116" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C116" s="11" t="s">
         <v>259</v>
@@ -28555,10 +28347,10 @@
     </row>
     <row r="117" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C117" s="11" t="s">
         <v>259</v>
@@ -28602,10 +28394,10 @@
     </row>
     <row r="118" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C118" s="11" t="s">
         <v>235</v>
@@ -28690,10 +28482,10 @@
     </row>
     <row r="120" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C120" s="11" t="s">
         <v>272</v>
@@ -28711,10 +28503,10 @@
     </row>
     <row r="121" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C121" s="11" t="s">
         <v>272</v>
@@ -29908,40 +29700,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>321</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>323</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -29958,28 +29750,28 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F2" t="s">
         <v>317</v>
       </c>
       <c r="G2" t="s">
+        <v>348</v>
+      </c>
+      <c r="H2" t="s">
         <v>349</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>334</v>
+      </c>
+      <c r="J2" t="s">
         <v>350</v>
       </c>
-      <c r="I2" t="s">
-        <v>335</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>351</v>
       </c>
-      <c r="K2" t="s">
-        <v>352</v>
-      </c>
       <c r="L2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -29996,28 +29788,28 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F3" t="s">
         <v>318</v>
       </c>
       <c r="G3" t="s">
+        <v>348</v>
+      </c>
+      <c r="H3" t="s">
         <v>349</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>334</v>
+      </c>
+      <c r="J3" t="s">
         <v>350</v>
       </c>
-      <c r="I3" t="s">
-        <v>335</v>
-      </c>
-      <c r="J3" t="s">
-        <v>351</v>
-      </c>
       <c r="K3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -30034,28 +29826,28 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F4" t="s">
         <v>317</v>
       </c>
       <c r="G4" t="s">
+        <v>354</v>
+      </c>
+      <c r="H4" t="s">
         <v>355</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>332</v>
+      </c>
+      <c r="J4" t="s">
         <v>356</v>
       </c>
-      <c r="I4" t="s">
-        <v>333</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>351</v>
+      </c>
+      <c r="L4" t="s">
         <v>357</v>
-      </c>
-      <c r="K4" t="s">
-        <v>352</v>
-      </c>
-      <c r="L4" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -30072,28 +29864,28 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F5" t="s">
         <v>317</v>
       </c>
       <c r="G5" t="s">
+        <v>358</v>
+      </c>
+      <c r="H5" t="s">
+        <v>355</v>
+      </c>
+      <c r="I5" t="s">
+        <v>332</v>
+      </c>
+      <c r="J5" t="s">
         <v>359</v>
       </c>
-      <c r="H5" t="s">
-        <v>356</v>
-      </c>
-      <c r="I5" t="s">
-        <v>333</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>360</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>361</v>
-      </c>
-      <c r="L5" t="s">
-        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -30134,22 +29926,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
+        <v>362</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>363</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="C1" s="46" t="s">
         <v>364</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>365</v>
       </c>
       <c r="D1" s="46" t="s">
         <v>324</v>
       </c>
       <c r="E1" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="F1" s="46" t="s">
         <v>366</v>
-      </c>
-      <c r="F1" s="46" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -30161,7 +29953,7 @@
         <v>true</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>17</v>
@@ -30188,7 +29980,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F3" s="45" t="s">
         <v>17</v>
@@ -30202,7 +29994,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F4" s="45" t="s">
         <v>15</v>
@@ -30210,7 +30002,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="45" t="s">

</xml_diff>